<commit_message>
probar archivo y arreglar micro errores
</commit_message>
<xml_diff>
--- a/Internacional/Rango proyecciones.xlsx
+++ b/Internacional/Rango proyecciones.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -30,16 +30,25 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00ffffff"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="008ba9d7"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -47,12 +56,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="00ffffff"/>
+      </left>
+      <right style="thin">
+        <color rgb="00ffffff"/>
+      </right>
+      <top style="thin">
+        <color rgb="00ffffff"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00ffffff"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -436,7 +462,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,29 +471,49 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Material</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Venta plan</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Stock planta</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Puerto Chile</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Centro Agua</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Puerto Oficina</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Almacen oficina</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Pesimista Proy.</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>Optimista. Proy.</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Pesimista Precio</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Optimista Precio</t>
         </is>
       </c>
     </row>
@@ -482,7 +528,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,29 +537,49 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Material</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Venta plan</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Stock planta</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Puerto Chile</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Centro Agua</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Puerto Oficina</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Almacen oficina</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Pesimista Proy.</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>Optimista. Proy.</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Pesimista Precio</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Optimista Precio</t>
         </is>
       </c>
     </row>
@@ -528,7 +594,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -537,29 +603,49 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Material</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Venta plan</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Stock planta</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Puerto Chile</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Centro Agua</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Puerto Oficina</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Almacen oficina</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Pesimista Proy.</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>Optimista. Proy.</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Pesimista Precio</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Optimista Precio</t>
         </is>
       </c>
     </row>
@@ -574,7 +660,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -583,29 +669,49 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Material</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Venta plan</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Stock planta</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Puerto Chile</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Centro Agua</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Puerto Oficina</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Almacen oficina</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Pesimista Proy.</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>Optimista. Proy.</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Pesimista Precio</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Optimista Precio</t>
         </is>
       </c>
     </row>
@@ -620,7 +726,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -629,29 +735,49 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Material</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Venta plan</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Stock planta</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Puerto Chile</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Centro Agua</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Puerto Oficina</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Almacen oficina</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Pesimista Proy.</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>Optimista. Proy.</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Pesimista Precio</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Optimista Precio</t>
         </is>
       </c>
     </row>

</xml_diff>